<commit_message>
Added excel of data from practise app
</commit_message>
<xml_diff>
--- a/steketid/empirical data.xlsx
+++ b/steketid/empirical data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\itsme\Dropbox\Dokumenter\Android_app\steketid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{46C79481-3405-4CDD-84CA-A659F65D501A}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8C4127-21F9-4E89-954A-93CF0EEE01B9}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" xr2:uid="{83595381-E7AD-4AA0-864F-F773C3218A6D}"/>
   </bookViews>
@@ -24,8 +24,31 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>time for next pizza</t>
+  </si>
+  <si>
+    <t>total time to cook one pizza</t>
+  </si>
+  <si>
+    <t>time through oven [min]</t>
+  </si>
+  <si>
+    <t>average [min]</t>
+  </si>
+  <si>
+    <t>total time for 5 pizzas</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="170" formatCode="mm:ss;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -55,8 +78,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,14 +395,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8DBD30D-36C6-4BDE-A69A-5A6BA2910BB9}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="20.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1.6550925925925926E-3</v>
+      </c>
+      <c r="B2" s="1">
+        <v>7.3032407407407412E-3</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1.462962962962963E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1.8865740740740742E-3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1.9212962962962962E-3</v>
+      </c>
+      <c r="B4">
+        <f>7 + 53/60</f>
+        <v>7.8833333333333329</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>1.8402777777777777E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f>2+38/60</f>
+        <v>2.6333333333333333</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>